<commit_message>
Mise à jour du dictionnaire de données
</commit_message>
<xml_diff>
--- a/Diagrammes/Dictionnaire_de_donnees.xlsx
+++ b/Diagrammes/Dictionnaire_de_donnees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoco\Documents\GitHub\Projet-POO-CPP-CLI\Diagrammes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6225E587-CE78-4886-B49A-8A88C41E8873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CB74AA-1A72-4DE2-87B7-EFB70A1F76CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8130" windowWidth="29040" windowHeight="15720" xr2:uid="{1312170F-3ACC-4C73-A594-411FC8B4E343}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1312170F-3ACC-4C73-A594-411FC8B4E343}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Entity</t>
   </si>
@@ -69,6 +69,63 @@
   </si>
   <si>
     <t>Primary Key - Identity (1,1)</t>
+  </si>
+  <si>
+    <t>People's Last Name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>Customer :</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>Customer's birth date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>People's First Name</t>
+  </si>
+  <si>
+    <t>first_order_date</t>
+  </si>
+  <si>
+    <t>Customer's first order date</t>
+  </si>
+  <si>
+    <t>Staff :</t>
+  </si>
+  <si>
+    <t>hiring_date</t>
+  </si>
+  <si>
+    <t>Staff's hiring date</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Address :</t>
   </si>
 </sst>
 </file>
@@ -420,14 +477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BA4FB3-8ECE-4430-97E3-603801167D9B}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -471,6 +530,157 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>225</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>225</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>